<commit_message>
Added Perceptron examples (major update).  Updated the README.md file.
</commit_message>
<xml_diff>
--- a/Lab4/Perceptron_Comparison.xlsx
+++ b/Lab4/Perceptron_Comparison.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="7">
   <si>
     <t>Ground Truth</t>
   </si>
@@ -25,13 +25,16 @@
     <t>Scikit Perceptron</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>R</t>
   </si>
   <si>
-    <t>M</t>
+    <t>Correct</t>
   </si>
   <si>
-    <t>Error</t>
+    <t>Mistake</t>
   </si>
 </sst>
 </file>
@@ -410,85 +413,181 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -499,72 +598,150 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -577,30 +754,60 @@
       <c r="A33" t="s">
         <v>3</v>
       </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>3</v>
       </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -611,12 +818,18 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -627,37 +840,73 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>3</v>
       </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>3</v>
       </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>4</v>
       </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
@@ -670,26 +919,56 @@
       <c r="A48" t="s">
         <v>3</v>
       </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>4</v>
       </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>4</v>
       </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
@@ -706,195 +985,423 @@
       <c r="A54" t="s">
         <v>3</v>
       </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>4</v>
       </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>4</v>
       </c>
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>4</v>
       </c>
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>4</v>
       </c>
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>3</v>
       </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>3</v>
       </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>3</v>
+      </c>
+      <c r="B80" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>4</v>
       </c>
+      <c r="B82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>3</v>
       </c>
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>4</v>
       </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>4</v>
       </c>
+      <c r="B85" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>4</v>
       </c>
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>3</v>
       </c>
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>3</v>
       </c>
+      <c r="B90" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
@@ -905,192 +1412,414 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>3</v>
       </c>
+      <c r="B94" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B95" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="B104" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="B108" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="B109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:1">
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B117" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B119" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B120" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B121" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B122" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B124" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B128" t="s">
+        <v>5</v>
+      </c>
+      <c r="C128" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>3</v>
       </c>
+      <c r="B129" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
@@ -1114,16 +1843,34 @@
       <c r="A132" t="s">
         <v>4</v>
       </c>
+      <c r="B132" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
         <v>3</v>
       </c>
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
         <v>4</v>
       </c>
+      <c r="B134" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
@@ -1140,20 +1887,38 @@
       <c r="A136" t="s">
         <v>4</v>
       </c>
+      <c r="B136" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
         <v>4</v>
       </c>
+      <c r="B137" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
         <v>4</v>
       </c>
+      <c r="B138" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B139" t="s">
         <v>5</v>
@@ -1164,32 +1929,68 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B141" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
         <v>4</v>
       </c>
+      <c r="B142" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
         <v>4</v>
       </c>
+      <c r="B144" t="s">
+        <v>5</v>
+      </c>
+      <c r="C144" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -1205,67 +2006,145 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B149" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B150" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
         <v>4</v>
       </c>
+      <c r="B151" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
         <v>4</v>
       </c>
+      <c r="B152" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
         <v>4</v>
       </c>
+      <c r="B153" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
         <v>3</v>
       </c>
+      <c r="B154" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
         <v>4</v>
       </c>
+      <c r="B155" t="s">
+        <v>5</v>
+      </c>
+      <c r="C155" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B156" t="s">
+        <v>5</v>
+      </c>
+      <c r="C156" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B157" t="s">
+        <v>5</v>
+      </c>
+      <c r="C157" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
         <v>4</v>
       </c>
+      <c r="B158" t="s">
+        <v>5</v>
+      </c>
+      <c r="C158" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B159" t="s">
+        <v>5</v>
+      </c>
+      <c r="C159" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -1279,175 +2158,361 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="B161" t="s">
+        <v>5</v>
+      </c>
+      <c r="C161" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B162" t="s">
+        <v>5</v>
+      </c>
+      <c r="C162" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="B163" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="B164" t="s">
+        <v>5</v>
+      </c>
+      <c r="C164" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B165" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
       <c r="A166" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="B166" t="s">
+        <v>5</v>
+      </c>
+      <c r="C166" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="168" spans="1:1">
+      <c r="B167" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B168" t="s">
+        <v>5</v>
+      </c>
+      <c r="C168" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
       <c r="A169" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="B169" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B171" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B172" t="s">
+        <v>5</v>
+      </c>
+      <c r="C172" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
       <c r="A173" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="B173" t="s">
+        <v>5</v>
+      </c>
+      <c r="C173" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1">
+        <v>3</v>
+      </c>
+      <c r="B174" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="B175" t="s">
+        <v>5</v>
+      </c>
+      <c r="C175" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
       <c r="A176" t="s">
         <v>4</v>
+      </c>
+      <c r="B176" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B177" t="s">
+        <v>5</v>
+      </c>
+      <c r="C177" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
         <v>4</v>
       </c>
+      <c r="B178" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B179" t="s">
+        <v>5</v>
+      </c>
+      <c r="C179" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
         <v>3</v>
       </c>
+      <c r="B180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C180" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C181" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B182" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
         <v>3</v>
       </c>
+      <c r="B183" t="s">
+        <v>5</v>
+      </c>
+      <c r="C183" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>5</v>
+      </c>
+      <c r="C184" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B185" t="s">
+        <v>5</v>
+      </c>
+      <c r="C185" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
         <v>4</v>
       </c>
+      <c r="B186" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B187" t="s">
+        <v>5</v>
+      </c>
+      <c r="C187" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B188" t="s">
+        <v>5</v>
+      </c>
+      <c r="C188" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
         <v>3</v>
       </c>
+      <c r="B189" t="s">
+        <v>5</v>
+      </c>
+      <c r="C189" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
         <v>3</v>
       </c>
+      <c r="B190" t="s">
+        <v>5</v>
+      </c>
+      <c r="C190" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B191" t="s">
+        <v>5</v>
+      </c>
+      <c r="C191" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
         <v>4</v>
       </c>
+      <c r="B192" t="s">
+        <v>5</v>
+      </c>
+      <c r="C192" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B193" t="s">
         <v>5</v>
@@ -1460,27 +2525,45 @@
       <c r="A194" t="s">
         <v>3</v>
       </c>
+      <c r="B194" t="s">
+        <v>5</v>
+      </c>
+      <c r="C194" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B195" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C195" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B196" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
         <v>4</v>
       </c>
+      <c r="B197" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
@@ -1495,58 +2578,112 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B199" t="s">
+        <v>5</v>
+      </c>
+      <c r="C199" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B200" t="s">
+        <v>5</v>
+      </c>
+      <c r="C200" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B201" t="s">
+        <v>5</v>
+      </c>
+      <c r="C201" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B202" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C202" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
         <v>3</v>
       </c>
+      <c r="B203" t="s">
+        <v>5</v>
+      </c>
+      <c r="C203" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
         <v>3</v>
       </c>
+      <c r="B204" t="s">
+        <v>5</v>
+      </c>
+      <c r="C204" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
         <v>4</v>
       </c>
+      <c r="B205" t="s">
+        <v>5</v>
+      </c>
+      <c r="C205" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B206" t="s">
+        <v>5</v>
+      </c>
+      <c r="C206" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
         <v>4</v>
       </c>
+      <c r="B207" t="s">
+        <v>6</v>
+      </c>
+      <c r="C207" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B208" t="s">
+        <v>5</v>
+      </c>
+      <c r="C208" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>